<commit_message>
LeaseForm: changing some stuff for easier import
</commit_message>
<xml_diff>
--- a/app/private/lease_import_v1.xlsx
+++ b/app/private/lease_import_v1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr date1904="1" showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2180" yWindow="0" windowWidth="25640" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27820" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="building_modele_import_building" sheetId="1" r:id="rId1"/>
@@ -1110,12 +1110,60 @@
         </r>
       </text>
     </comment>
+    <comment ref="BQ1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+good, average, bad</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EO1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Commentaires généraux</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="168">
   <si>
     <t>building_id</t>
   </si>
@@ -1397,6 +1445,228 @@
   </si>
   <si>
     <t>Ceci est un autre commentaire</t>
+  </si>
+  <si>
+    <t>comfort_qualitative_assessment.acoustic</t>
+  </si>
+  <si>
+    <t>comfort_qualitative_assessment.visual</t>
+  </si>
+  <si>
+    <t>comfort_qualitative_assessment.thermic</t>
+  </si>
+  <si>
+    <t>comfort_qualitative_assessment.comments</t>
+  </si>
+  <si>
+    <t>technical_compliance.0.name</t>
+  </si>
+  <si>
+    <t>technical_compliance.0.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.0.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.0.description</t>
+  </si>
+  <si>
+    <t>Structure</t>
+  </si>
+  <si>
+    <t>technical_compliance.tc_comments</t>
+  </si>
+  <si>
+    <t>technical_compliance.1.name</t>
+  </si>
+  <si>
+    <t>technical_compliance.1.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.1.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.1.description</t>
+  </si>
+  <si>
+    <t>technical_compliance.2.name</t>
+  </si>
+  <si>
+    <t>technical_compliance.2.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.2.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.2.description</t>
+  </si>
+  <si>
+    <t>technical_compliance.3.name</t>
+  </si>
+  <si>
+    <t>technical_compliance.3.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.3.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.3.description</t>
+  </si>
+  <si>
+    <t>technical_compliance.4.name</t>
+  </si>
+  <si>
+    <t>technical_compliance.4.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.4.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.4.description</t>
+  </si>
+  <si>
+    <t>technical_compliance.5.name</t>
+  </si>
+  <si>
+    <t>technical_compliance.5.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.5.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.5.description</t>
+  </si>
+  <si>
+    <t>technical_compliance.6.name</t>
+  </si>
+  <si>
+    <t>technical_compliance.6.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.6.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.6.description</t>
+  </si>
+  <si>
+    <t>technical_compliance.7.name</t>
+  </si>
+  <si>
+    <t>technical_compliance.7.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.7.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.7.description</t>
+  </si>
+  <si>
+    <t>technical_compliance.8.name</t>
+  </si>
+  <si>
+    <t>technical_compliance.8.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.8.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.8.description</t>
+  </si>
+  <si>
+    <t>technical_compliance.9.name</t>
+  </si>
+  <si>
+    <t>technical_compliance.9.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.9.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.9.description</t>
+  </si>
+  <si>
+    <t>technical_compliance.10.name</t>
+  </si>
+  <si>
+    <t>technical_compliance.11.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.10.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.10.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.10.description</t>
+  </si>
+  <si>
+    <t>technical_compliance.11.name</t>
+  </si>
+  <si>
+    <t>technical_compliance.11.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.11.description</t>
+  </si>
+  <si>
+    <t>technical_compliance.12.name</t>
+  </si>
+  <si>
+    <t>technical_compliance.13.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.14.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.12.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.12.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.12.description</t>
+  </si>
+  <si>
+    <t>technical_compliance.13.name</t>
+  </si>
+  <si>
+    <t>technical_compliance.13.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.13.description</t>
+  </si>
+  <si>
+    <t>technical_compliance.14.name</t>
+  </si>
+  <si>
+    <t>technical_compliance.14.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.14.description</t>
+  </si>
+  <si>
+    <t>technical_compliance.15.name</t>
+  </si>
+  <si>
+    <t>technical_compliance.15.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.15.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.15.description</t>
+  </si>
+  <si>
+    <t>technical_compliance.16.name</t>
+  </si>
+  <si>
+    <t>technical_compliance.16.lifetime</t>
+  </si>
+  <si>
+    <t>technical_compliance.16.conformity</t>
+  </si>
+  <si>
+    <t>technical_compliance.16.description</t>
   </si>
 </sst>
 </file>
@@ -1488,8 +1758,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1552,7 +1842,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="41">
+  <cellStyles count="61">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -1573,6 +1863,16 @@
     <cellStyle name="Lien hypertexte" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -1593,6 +1893,16 @@
     <cellStyle name="Lien hypertexte visité" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1923,10 +2233,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:BP2"/>
+  <dimension ref="A1:EO2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BI1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="BP3" sqref="BP3"/>
+    <sheetView tabSelected="1" topLeftCell="EB1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="EJ1" sqref="EG1:EJ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1997,9 +2307,82 @@
     <col min="66" max="66" width="17.83203125" customWidth="1"/>
     <col min="67" max="67" width="13.5" customWidth="1"/>
     <col min="68" max="68" width="17.83203125" customWidth="1"/>
+    <col min="69" max="69" width="20.5" customWidth="1"/>
+    <col min="70" max="70" width="19.33203125" customWidth="1"/>
+    <col min="71" max="71" width="19.1640625" customWidth="1"/>
+    <col min="72" max="72" width="19.5" customWidth="1"/>
+    <col min="73" max="73" width="18.6640625" customWidth="1"/>
+    <col min="74" max="74" width="18.5" customWidth="1"/>
+    <col min="75" max="75" width="18.83203125" customWidth="1"/>
+    <col min="76" max="76" width="18.5" customWidth="1"/>
+    <col min="77" max="77" width="18.6640625" customWidth="1"/>
+    <col min="78" max="78" width="18.5" customWidth="1"/>
+    <col min="79" max="79" width="18.83203125" customWidth="1"/>
+    <col min="80" max="80" width="18.5" customWidth="1"/>
+    <col min="81" max="81" width="18.6640625" customWidth="1"/>
+    <col min="82" max="82" width="18.5" customWidth="1"/>
+    <col min="83" max="83" width="18.83203125" customWidth="1"/>
+    <col min="84" max="84" width="18.5" customWidth="1"/>
+    <col min="85" max="85" width="18.6640625" customWidth="1"/>
+    <col min="86" max="86" width="18.5" customWidth="1"/>
+    <col min="87" max="87" width="18.83203125" customWidth="1"/>
+    <col min="88" max="88" width="18.5" customWidth="1"/>
+    <col min="89" max="89" width="18.6640625" customWidth="1"/>
+    <col min="90" max="90" width="18.5" customWidth="1"/>
+    <col min="91" max="91" width="18.83203125" customWidth="1"/>
+    <col min="92" max="92" width="18.5" customWidth="1"/>
+    <col min="93" max="93" width="18.6640625" customWidth="1"/>
+    <col min="94" max="94" width="18.5" customWidth="1"/>
+    <col min="95" max="95" width="18.83203125" customWidth="1"/>
+    <col min="96" max="96" width="18.5" customWidth="1"/>
+    <col min="97" max="97" width="18.6640625" customWidth="1"/>
+    <col min="98" max="98" width="18.5" customWidth="1"/>
+    <col min="99" max="99" width="18.83203125" customWidth="1"/>
+    <col min="100" max="100" width="18.5" customWidth="1"/>
+    <col min="101" max="101" width="18.6640625" customWidth="1"/>
+    <col min="102" max="102" width="18.5" customWidth="1"/>
+    <col min="103" max="103" width="18.83203125" customWidth="1"/>
+    <col min="104" max="104" width="18.5" customWidth="1"/>
+    <col min="105" max="105" width="18.6640625" customWidth="1"/>
+    <col min="106" max="106" width="18.5" customWidth="1"/>
+    <col min="107" max="107" width="18.83203125" customWidth="1"/>
+    <col min="108" max="108" width="18.5" customWidth="1"/>
+    <col min="109" max="109" width="18.6640625" customWidth="1"/>
+    <col min="110" max="110" width="18.5" customWidth="1"/>
+    <col min="111" max="111" width="18.83203125" customWidth="1"/>
+    <col min="112" max="112" width="18.5" customWidth="1"/>
+    <col min="113" max="113" width="18.6640625" customWidth="1"/>
+    <col min="114" max="114" width="18.5" customWidth="1"/>
+    <col min="115" max="115" width="18.83203125" customWidth="1"/>
+    <col min="116" max="116" width="18.5" customWidth="1"/>
+    <col min="117" max="117" width="18.6640625" customWidth="1"/>
+    <col min="118" max="118" width="18.5" customWidth="1"/>
+    <col min="119" max="119" width="18.83203125" customWidth="1"/>
+    <col min="120" max="120" width="18.5" customWidth="1"/>
+    <col min="121" max="121" width="18.6640625" customWidth="1"/>
+    <col min="122" max="122" width="18.5" customWidth="1"/>
+    <col min="123" max="123" width="18.83203125" customWidth="1"/>
+    <col min="124" max="124" width="18.5" customWidth="1"/>
+    <col min="125" max="125" width="18.6640625" customWidth="1"/>
+    <col min="126" max="126" width="18.5" customWidth="1"/>
+    <col min="127" max="127" width="18.83203125" customWidth="1"/>
+    <col min="128" max="128" width="18.5" customWidth="1"/>
+    <col min="129" max="129" width="18.6640625" customWidth="1"/>
+    <col min="130" max="130" width="18.5" customWidth="1"/>
+    <col min="131" max="131" width="18.83203125" customWidth="1"/>
+    <col min="132" max="132" width="18.5" customWidth="1"/>
+    <col min="133" max="133" width="18.6640625" customWidth="1"/>
+    <col min="134" max="134" width="18.5" customWidth="1"/>
+    <col min="135" max="135" width="18.83203125" customWidth="1"/>
+    <col min="136" max="136" width="18.5" customWidth="1"/>
+    <col min="137" max="137" width="18.6640625" customWidth="1"/>
+    <col min="138" max="138" width="18.5" customWidth="1"/>
+    <col min="139" max="139" width="18.83203125" customWidth="1"/>
+    <col min="140" max="140" width="18.5" customWidth="1"/>
+    <col min="145" max="145" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" s="1" customFormat="1" ht="30">
+    <row r="1" spans="1:145" s="1" customFormat="1" ht="30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2204,8 +2587,227 @@
       <c r="BP1" s="1" t="s">
         <v>90</v>
       </c>
+      <c r="BQ1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="BR1" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="BS1" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="BT1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="BU1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="BW1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="BX1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="BY1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="BZ1" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="CA1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="CB1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="CC1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="CD1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="CE1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="CF1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="CG1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="CH1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="CI1" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="CJ1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="CK1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="CL1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="CM1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="CN1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="CO1" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="CP1" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="CQ1" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="CR1" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="CS1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="CT1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="CU1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="CV1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="CW1" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="CX1" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="CY1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="CZ1" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="DA1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="DB1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="DC1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="DD1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="DE1" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="DF1" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="DG1" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="DH1" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="DI1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="DJ1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="DK1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="DL1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="DM1" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="DN1" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="DO1" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="DP1" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="DQ1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="DR1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="DS1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="DT1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="DU1" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="DV1" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="DW1" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="DX1" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="DY1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="DZ1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="EA1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="EB1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="EC1" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="ED1" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="EE1" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="EF1" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="EG1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="EH1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="EI1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="EJ1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="EO1" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
-    <row r="2" spans="1:68" s="2" customFormat="1" ht="30">
+    <row r="2" spans="1:145" s="2" customFormat="1" ht="30">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -2370,6 +2972,41 @@
       </c>
       <c r="BO2" s="2" t="s">
         <v>92</v>
+      </c>
+      <c r="BU2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="BY2" s="6"/>
+      <c r="CC2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="CG2" s="6"/>
+      <c r="CK2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="CO2" s="6"/>
+      <c r="CS2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="CW2" s="6"/>
+      <c r="DA2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="DE2" s="6"/>
+      <c r="DI2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="DM2" s="6"/>
+      <c r="DQ2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="DU2" s="6"/>
+      <c r="DY2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="EC2" s="6"/>
+      <c r="EG2" s="6" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small changes + moving quick-delete warging as a global helper
</commit_message>
<xml_diff>
--- a/app/private/lease_import_v1.xlsx
+++ b/app/private/lease_import_v1.xlsx
@@ -1134,6 +1134,438 @@
         </r>
       </text>
     </comment>
+    <comment ref="BV1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+new_dvr, good_dvr, average_dvr, bad_dvr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BW1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+compliant, not_compliant_minor, not_compliant_major</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BZ1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+new_dvr, good_dvr, average_dvr, bad_dvr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CA1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+compliant, not_compliant_minor, not_compliant_major</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CD1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+new_dvr, good_dvr, average_dvr, bad_dvr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CE1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+compliant, not_compliant_minor, not_compliant_major</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CH1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+new_dvr, good_dvr, average_dvr, bad_dvr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CI1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+compliant, not_compliant_minor, not_compliant_major</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CL1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+new_dvr, good_dvr, average_dvr, bad_dvr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CM1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+compliant, not_compliant_minor, not_compliant_major</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CP1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+new_dvr, good_dvr, average_dvr, bad_dvr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CQ1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+compliant, not_compliant_minor, not_compliant_major</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CT1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+new_dvr, good_dvr, average_dvr, bad_dvr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CU1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+compliant, not_compliant_minor, not_compliant_major</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EK1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Commentaires généraux</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EL1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+true, false</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EM1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+monthly, quaterly, bi_annual, yearly, 2_years, 5_years, 7_years, 10_years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EN1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Ex : 2014-12-20</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="EO1" authorId="0">
       <text>
         <r>
@@ -1154,7 +1586,1255 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Commentaires généraux</t>
+compliant, not_compliant_minor, not_compliant_major</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EQ1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+true, false</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="ER1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+monthly, quaterly, bi_annual, yearly, 2_years, 5_years, 7_years, 10_years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="ES1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Ex : 2014-12-20</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="ET1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+compliant, not_compliant_minor, not_compliant_major</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EV1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+true, false</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EW1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+monthly, quaterly, bi_annual, yearly, 2_years, 5_years, 7_years, 10_years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EX1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Ex : 2014-12-20</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="EY1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+compliant, not_compliant_minor, not_compliant_major</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="FA1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+true, false</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="FB1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+monthly, quaterly, bi_annual, yearly, 2_years, 5_years, 7_years, 10_years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="FC1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Ex : 2014-12-20</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="FD1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+compliant, not_compliant_minor, not_compliant_major</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="FF1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+true, false</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="FG1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+monthly, quaterly, bi_annual, yearly, 2_years, 5_years, 7_years, 10_years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="FH1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Ex : 2014-12-20</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="FI1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+compliant, not_compliant_minor, not_compliant_major</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="FK1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+true, false</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="FL1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+monthly, quaterly, bi_annual, yearly, 2_years, 5_years, 7_years, 10_years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="FM1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Ex : 2014-12-20</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="FN1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+compliant, not_compliant_minor, not_compliant_major</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="FP1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+true, false</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="FQ1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+monthly, quaterly, bi_annual, yearly, 2_years, 5_years, 7_years, 10_years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="FR1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Ex : 2014-12-20</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="FS1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+compliant, not_compliant_minor, not_compliant_major</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="FU1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+true, false</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="FV1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+monthly, quaterly, bi_annual, yearly, 2_years, 5_years, 7_years, 10_years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="FW1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Ex : 2014-12-20</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="FX1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+compliant, not_compliant_minor, not_compliant_major</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="FZ1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+true, false</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="GA1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+monthly, quaterly, bi_annual, yearly, 2_years, 5_years, 7_years, 10_years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="GB1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Ex : 2014-12-20</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="GC1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+compliant, not_compliant_minor, not_compliant_major</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="GE1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+true, false</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="GF1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+monthly, quaterly, bi_annual, yearly, 2_years, 5_years, 7_years, 10_years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="GG1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Ex : 2014-12-20</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="GH1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+compliant, not_compliant_minor, not_compliant_major</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="GJ1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+true, false</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="GK1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+monthly, quaterly, bi_annual, yearly, 2_years, 5_years, 7_years, 10_years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="GL1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Ex : 2014-12-20</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="GM1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+compliant, not_compliant_minor, not_compliant_major</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="GO1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+true, false</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="GP1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+monthly, quaterly, bi_annual, yearly, 2_years, 5_years, 7_years, 10_years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="GQ1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Ex : 2014-12-20</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="GR1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+compliant, not_compliant_minor, not_compliant_major</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="GT1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+true, false</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="GU1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+monthly, quaterly, bi_annual, yearly, 2_years, 5_years, 7_years, 10_years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="GV1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Ex : 2014-12-20</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="GW1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+compliant, not_compliant_minor, not_compliant_major</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="GY1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+true, false</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="GZ1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+monthly, quaterly, bi_annual, yearly, 2_years, 5_years, 7_years, 10_years</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="HA1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Ex : 2014-12-20</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="HB1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Benjamin-Samuel Ewenczyk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+compliant, not_compliant_minor, not_compliant_major</t>
         </r>
       </text>
     </comment>
@@ -1163,7 +2843,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="258">
   <si>
     <t>building_id</t>
   </si>
@@ -1667,6 +3347,276 @@
   </si>
   <si>
     <t>technical_compliance.16.description</t>
+  </si>
+  <si>
+    <t>Facade</t>
+  </si>
+  <si>
+    <t>Toiture / étanchéité</t>
+  </si>
+  <si>
+    <t>Production Chaud</t>
+  </si>
+  <si>
+    <t>Production Froid</t>
+  </si>
+  <si>
+    <t>TGBT</t>
+  </si>
+  <si>
+    <t>Distribution électrique</t>
+  </si>
+  <si>
+    <t>Distribution thermique</t>
+  </si>
+  <si>
+    <t>Terminaux chauffage</t>
+  </si>
+  <si>
+    <t>Terminaux climatisation</t>
+  </si>
+  <si>
+    <t>Terminaux d'éclairage</t>
+  </si>
+  <si>
+    <t>GTC/GTB</t>
+  </si>
+  <si>
+    <t>Centrales d'air</t>
+  </si>
+  <si>
+    <t>Réseaux ventilation</t>
+  </si>
+  <si>
+    <t>Production ECS</t>
+  </si>
+  <si>
+    <t>Distribution ECS</t>
+  </si>
+  <si>
+    <t>Sécurité incendie</t>
+  </si>
+  <si>
+    <t>accessibility.eligibility</t>
+  </si>
+  <si>
+    <t>accessibility.periodicity</t>
+  </si>
+  <si>
+    <t>accessibility.due_date</t>
+  </si>
+  <si>
+    <t>2014-12-20</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>7_years</t>
+  </si>
+  <si>
+    <t>accessibility.conformity</t>
+  </si>
+  <si>
+    <t>accessibility.description</t>
+  </si>
+  <si>
+    <t>compliant</t>
+  </si>
+  <si>
+    <t>elevators.eligibility</t>
+  </si>
+  <si>
+    <t>elevators.periodicity</t>
+  </si>
+  <si>
+    <t>elevators.due_date</t>
+  </si>
+  <si>
+    <t>elevators.conformity</t>
+  </si>
+  <si>
+    <t>elevators.description</t>
+  </si>
+  <si>
+    <t>ssi.eligibility</t>
+  </si>
+  <si>
+    <t>ssi.periodicity</t>
+  </si>
+  <si>
+    <t>ssi.due_date</t>
+  </si>
+  <si>
+    <t>ssi.conformity</t>
+  </si>
+  <si>
+    <t>ssi.description</t>
+  </si>
+  <si>
+    <t>asbestos.eligibility</t>
+  </si>
+  <si>
+    <t>asbestos.periodicity</t>
+  </si>
+  <si>
+    <t>asbestos.due_date</t>
+  </si>
+  <si>
+    <t>asbestos.conformity</t>
+  </si>
+  <si>
+    <t>asbestos.description</t>
+  </si>
+  <si>
+    <t>lead.eligibility</t>
+  </si>
+  <si>
+    <t>lead.periodicity</t>
+  </si>
+  <si>
+    <t>lead.due_date</t>
+  </si>
+  <si>
+    <t>lead.conformity</t>
+  </si>
+  <si>
+    <t>lead.description</t>
+  </si>
+  <si>
+    <t>legionella.eligibility</t>
+  </si>
+  <si>
+    <t>legionella.periodicity</t>
+  </si>
+  <si>
+    <t>legionella.due_date</t>
+  </si>
+  <si>
+    <t>legionella.conformity</t>
+  </si>
+  <si>
+    <t>legionella.description</t>
+  </si>
+  <si>
+    <t>electrical_installation.eligibility</t>
+  </si>
+  <si>
+    <t>electrical_installation.periodicity</t>
+  </si>
+  <si>
+    <t>electrical_installation.due_date</t>
+  </si>
+  <si>
+    <t>electrical_installation.conformity</t>
+  </si>
+  <si>
+    <t>electrical_installation.description</t>
+  </si>
+  <si>
+    <t>dpe.eligibility</t>
+  </si>
+  <si>
+    <t>dpe.periodicity</t>
+  </si>
+  <si>
+    <t>dpe.due_date</t>
+  </si>
+  <si>
+    <t>dpe.conformity</t>
+  </si>
+  <si>
+    <t>dpe.description</t>
+  </si>
+  <si>
+    <t>indoor_air_quality.eligibility</t>
+  </si>
+  <si>
+    <t>indoor_air_quality.periodicity</t>
+  </si>
+  <si>
+    <t>indoor_air_quality.due_date</t>
+  </si>
+  <si>
+    <t>indoor_air_quality.conformity</t>
+  </si>
+  <si>
+    <t>indoor_air_quality.description</t>
+  </si>
+  <si>
+    <t>radon.eligibility</t>
+  </si>
+  <si>
+    <t>radon.periodicity</t>
+  </si>
+  <si>
+    <t>radon.due_date</t>
+  </si>
+  <si>
+    <t>radon.conformity</t>
+  </si>
+  <si>
+    <t>radon.description</t>
+  </si>
+  <si>
+    <t>chiller_terminal.eligibility</t>
+  </si>
+  <si>
+    <t>chiller_terminal.periodicity</t>
+  </si>
+  <si>
+    <t>chiller_terminal.due_date</t>
+  </si>
+  <si>
+    <t>chiller_terminal.conformity</t>
+  </si>
+  <si>
+    <t>chiller_terminal.description</t>
+  </si>
+  <si>
+    <t>lead_disconnector.eligibility</t>
+  </si>
+  <si>
+    <t>lead_disconnector.periodicity</t>
+  </si>
+  <si>
+    <t>lead_disconnector.due_date</t>
+  </si>
+  <si>
+    <t>lead_disconnector.conformity</t>
+  </si>
+  <si>
+    <t>lead_disconnector.description</t>
+  </si>
+  <si>
+    <t>automatic_doors.eligibility</t>
+  </si>
+  <si>
+    <t>automatic_doors.periodicity</t>
+  </si>
+  <si>
+    <t>automatic_doors.due_date</t>
+  </si>
+  <si>
+    <t>automatic_doors.conformity</t>
+  </si>
+  <si>
+    <t>automatic_doors.description</t>
+  </si>
+  <si>
+    <t>chiller_system.eligibility</t>
+  </si>
+  <si>
+    <t>chiller_system.periodicity</t>
+  </si>
+  <si>
+    <t>chiller_system.due_date</t>
+  </si>
+  <si>
+    <t>chiller_system.conformity</t>
+  </si>
+  <si>
+    <t>chiller_system.description</t>
   </si>
 </sst>
 </file>
@@ -1758,7 +3708,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="61">
+  <cellStyleXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1820,8 +3770,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1841,8 +3807,11 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="61">
+  <cellStyles count="77">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -1873,6 +3842,14 @@
     <cellStyle name="Lien hypertexte" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -1903,6 +3880,14 @@
     <cellStyle name="Lien hypertexte visité" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2233,10 +4218,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:EO2"/>
+  <dimension ref="A1:HC2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="EB1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="EJ1" sqref="EG1:EJ1"/>
+    <sheetView tabSelected="1" topLeftCell="GT1" workbookViewId="0">
+      <selection activeCell="HA19" sqref="HA19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2379,10 +4364,11 @@
     <col min="138" max="138" width="18.5" customWidth="1"/>
     <col min="139" max="139" width="18.83203125" customWidth="1"/>
     <col min="140" max="140" width="18.5" customWidth="1"/>
-    <col min="145" max="145" width="16.6640625" customWidth="1"/>
+    <col min="141" max="141" width="16.6640625" customWidth="1"/>
+    <col min="142" max="211" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:145" s="1" customFormat="1" ht="30">
+    <row r="1" spans="1:211" s="1" customFormat="1" ht="30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2803,11 +4789,221 @@
       <c r="EJ1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="EO1" s="1" t="s">
+      <c r="EK1" s="3" t="s">
         <v>103</v>
       </c>
+      <c r="EL1" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="EM1" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="EN1" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="EO1" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="EP1" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="EQ1" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="ER1" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="ES1" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="ET1" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="EU1" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="EV1" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="EW1" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="EX1" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="EY1" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="EZ1" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="FA1" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="FB1" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="FC1" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="FD1" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="FE1" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="FF1" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="FG1" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="FH1" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="FI1" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="FJ1" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="FK1" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="FL1" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="FM1" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="FN1" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="FO1" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="FP1" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="FQ1" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="FR1" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="FS1" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="FT1" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="FU1" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="FV1" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="FW1" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="FX1" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="FY1" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="FZ1" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="GA1" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="GB1" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="GC1" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="GD1" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="GE1" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="GF1" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="GG1" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="GH1" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="GI1" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="GJ1" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="GK1" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="GL1" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="GM1" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="GN1" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="GO1" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="GP1" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="GQ1" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="GR1" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="GS1" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="GT1" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="GU1" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="GV1" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="GW1" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="GX1" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="GY1" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="GZ1" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="HA1" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="HB1" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="HC1" s="5" t="s">
+        <v>257</v>
+      </c>
     </row>
-    <row r="2" spans="1:145" s="2" customFormat="1" ht="30">
+    <row r="2" spans="1:211" s="2" customFormat="1" ht="30">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -2976,37 +5172,221 @@
       <c r="BU2" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="BY2" s="6"/>
+      <c r="BY2" s="6" t="s">
+        <v>168</v>
+      </c>
       <c r="CC2" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="CG2" s="6"/>
+        <v>169</v>
+      </c>
+      <c r="CG2" s="6" t="s">
+        <v>170</v>
+      </c>
       <c r="CK2" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="CO2" s="6"/>
+        <v>171</v>
+      </c>
+      <c r="CO2" s="6" t="s">
+        <v>172</v>
+      </c>
       <c r="CS2" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="CW2" s="6"/>
+        <v>173</v>
+      </c>
+      <c r="CW2" s="6" t="s">
+        <v>174</v>
+      </c>
       <c r="DA2" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="DE2" s="6"/>
+        <v>175</v>
+      </c>
+      <c r="DE2" s="6" t="s">
+        <v>176</v>
+      </c>
       <c r="DI2" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="DM2" s="6"/>
+        <v>177</v>
+      </c>
+      <c r="DM2" s="6" t="s">
+        <v>178</v>
+      </c>
       <c r="DQ2" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="DU2" s="6"/>
+        <v>179</v>
+      </c>
+      <c r="DU2" s="6" t="s">
+        <v>180</v>
+      </c>
       <c r="DY2" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="EC2" s="6"/>
+        <v>181</v>
+      </c>
+      <c r="EC2" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="EG2" s="6" t="s">
-        <v>102</v>
+        <v>183</v>
+      </c>
+      <c r="EL2" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="EM2" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="EN2" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="EO2" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="EQ2" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="ER2" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="ES2" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="ET2" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="EV2" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="EW2" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="EX2" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="EY2" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="FA2" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="FB2" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="FC2" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="FD2" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="FF2" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="FG2" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="FH2" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="FI2" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="FK2" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="FL2" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="FM2" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="FN2" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="FP2" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="FQ2" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="FR2" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="FS2" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="FU2" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="FV2" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="FW2" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="FX2" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="FZ2" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="GA2" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="GB2" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="GC2" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="GE2" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="GF2" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="GG2" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="GH2" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="GJ2" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="GK2" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="GL2" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="GM2" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="GO2" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="GP2" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="GQ2" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="GR2" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="GT2" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="GU2" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="GV2" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="GW2" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="GY2" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="GZ2" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="HA2" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="HB2" s="2" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>